<commit_message>
update : burndown chart
</commit_message>
<xml_diff>
--- a/BurndownSAE.xlsx
+++ b/BurndownSAE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/curiosow/Documents/Cours/BUT2/SAE-EMPLOIDUTEMPS/SAE3.01/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aephy\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FB61E1-E84A-6448-A0CE-DB18568005AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358A7AF6-B592-42B7-A439-A5AE88041A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16800" xr2:uid="{3DD71429-2E7F-4DAC-A99F-E3D1D95592DF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3DD71429-2E7F-4DAC-A99F-E3D1D95592DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -172,7 +172,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -236,6 +236,9 @@
                   <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>42</c:v>
                 </c:pt>
               </c:numCache>
@@ -323,6 +326,9 @@
                 <c:pt idx="7">
                   <c:v>42</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>42</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -338,6 +344,9 @@
                 <c:pt idx="1">
                   <c:v>42</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>42</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -349,6 +358,7 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -401,7 +411,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="25048352"/>
@@ -460,7 +470,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="25050272"/>
@@ -475,6 +485,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -501,7 +542,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -515,7 +556,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -577,7 +618,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -654,6 +695,9 @@
                 <c:pt idx="2">
                   <c:v>23</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -725,6 +769,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -789,7 +836,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2021162991"/>
@@ -848,7 +895,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2021153391"/>
@@ -890,7 +937,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -920,7 +967,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2427,12 +2474,12 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2455,7 +2502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2472,7 +2519,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2490,26 +2537,35 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
         <v>23</v>
       </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>42</v>
+      </c>
       <c r="F4">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
       <c r="F5">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2517,7 +2573,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>

</xml_diff>